<commit_message>
vierde iteratie gedaan, vijfde staat klaar
</commit_message>
<xml_diff>
--- a/Identifier/Old to label/to_label3.xlsx
+++ b/Identifier/Old to label/to_label3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jefva\Documents\Master\Thesis_s2\Code\Identifier\Old to label\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3C1A29-3C01-42ED-BA66-5D91C62AAA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A54ECC-BD12-4105-9CE4-A75FD06C7192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -963,7 +963,7 @@
   <dimension ref="A1:E202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B201"/>
+      <selection activeCell="C203" sqref="C203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>